<commit_message>
prepared output files for all runs
</commit_message>
<xml_diff>
--- a/spine_projects/03_output_data/02_runs_EURO/02_output_prepared/output_LCOE_overview.xlsx
+++ b/spine_projects/03_output_data/02_runs_EURO/02_output_prepared/output_LCOE_overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\03_output_data\02_runs_EURO\02_output_prepared\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F17034F-1613-464B-8978-DCF652C65580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F7C86D-FED4-4B95-8688-E6D3FB602DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>run_name</t>
   </si>
@@ -46,7 +46,10 @@
     <t>pcf_value</t>
   </si>
   <si>
-    <t>base</t>
+    <t>base_case</t>
+  </si>
+  <si>
+    <t>base_case_PV</t>
   </si>
 </sst>
 </file>
@@ -412,7 +415,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -471,7 +474,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>160.7303598307972</v>

</xml_diff>